<commit_message>
Small fix on first sheet
</commit_message>
<xml_diff>
--- a/test-analysis/hackathon-netcompany-auth-test-analysis-team21_2023_12_20.xlsx
+++ b/test-analysis/hackathon-netcompany-auth-test-analysis-team21_2023_12_20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fttolias\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FF0557-50DA-4C3B-AACA-169267E6888F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D324CC1-1464-4AA8-B31B-535B8CD5DEBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Report" sheetId="1" r:id="rId1"/>
@@ -842,19 +842,19 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1088,19 +1088,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2"/>
@@ -1126,13 +1126,13 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1159,7 +1159,7 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="31">
         <v>45282</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1193,7 +1193,7 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="31">
         <v>45282</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1227,7 +1227,7 @@
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="31">
         <v>45282</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1263,7 +1263,7 @@
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="31">
         <v>45282</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1299,7 +1299,7 @@
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="31">
         <v>45282</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1333,7 +1333,7 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="31">
         <v>45282</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1367,7 +1367,7 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="31">
         <v>45282</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1403,7 +1403,7 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="31">
         <v>45282</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1439,14 +1439,14 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="31">
         <v>45282</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D11" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
@@ -1475,7 +1475,7 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="31">
         <v>45282</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1509,7 +1509,7 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="31">
         <v>45282</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1543,7 +1543,7 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="31">
         <v>45282</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1577,7 +1577,7 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="31">
         <v>45282</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1611,7 +1611,7 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="31">
         <v>45282</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1645,7 +1645,7 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="31">
         <v>45282</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1681,7 +1681,7 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="31">
         <v>45282</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1715,7 +1715,7 @@
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="31">
         <v>45282</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -1749,7 +1749,7 @@
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="36">
+      <c r="B20" s="31">
         <v>45282</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1783,7 +1783,7 @@
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="36">
+      <c r="B21" s="31">
         <v>45282</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -29241,7 +29241,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -29258,10 +29260,10 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>1</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -29273,10 +29275,10 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -29288,10 +29290,10 @@
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
@@ -29303,10 +29305,10 @@
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -29318,10 +29320,10 @@
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
@@ -29380,10 +29382,10 @@
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="36">
         <v>2</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="E10" s="6" t="s">
         <v>3</v>
       </c>
@@ -29395,10 +29397,10 @@
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="E11" s="8" t="s">
         <v>8</v>
       </c>
@@ -29410,10 +29412,10 @@
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="E12" s="8" t="s">
         <v>0</v>
       </c>
@@ -29425,10 +29427,10 @@
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
@@ -29440,10 +29442,10 @@
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="34"/>
+      <c r="C14" s="35"/>
       <c r="E14" s="8" t="s">
         <v>18</v>
       </c>
@@ -29585,20 +29587,20 @@
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="33">
+      <c r="B27" s="36">
         <v>3</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="35"/>
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
@@ -29608,10 +29610,10 @@
       <c r="A29" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="E29" s="8" t="s">
         <v>8</v>
       </c>
@@ -29621,10 +29623,10 @@
       <c r="A30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="E30" s="8" t="s">
         <v>0</v>
       </c>
@@ -29634,10 +29636,10 @@
       <c r="A31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="E31" s="8" t="s">
         <v>14</v>
       </c>
@@ -29725,50 +29727,50 @@
       <c r="A39" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="33">
+      <c r="B39" s="36">
         <v>4</v>
       </c>
-      <c r="C39" s="34"/>
+      <c r="C39" s="35"/>
       <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:23" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="34"/>
+      <c r="C40" s="35"/>
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:23" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="34"/>
+      <c r="C41" s="35"/>
       <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:23" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="34"/>
+      <c r="C42" s="35"/>
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:23" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="34"/>
+      <c r="C43" s="35"/>
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:23" ht="15.75" customHeight="1">
@@ -29861,24 +29863,24 @@
       <c r="A55" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="34"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
       <c r="F55" s="13"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
       <c r="A56" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35"/>
       <c r="F56" s="13"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="34"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="35"/>
       <c r="F57" s="13"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1">
@@ -29955,24 +29957,24 @@
       <c r="A68" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="35"/>
       <c r="F68" s="13"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" customHeight="1">
       <c r="A69" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B69" s="35"/>
-      <c r="C69" s="34"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="35"/>
       <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1">
       <c r="A70" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="35"/>
       <c r="F70" s="13"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1">
@@ -32818,6 +32820,21 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B69:C69"/>
@@ -32829,21 +32846,6 @@
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -32859,7 +32861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F989"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -32878,10 +32880,10 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>5</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -32893,10 +32895,10 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -32908,10 +32910,10 @@
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
@@ -32923,10 +32925,10 @@
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -32938,10 +32940,10 @@
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
@@ -33056,10 +33058,10 @@
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="36">
         <v>6</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="E18" s="6" t="s">
         <v>3</v>
       </c>
@@ -33071,10 +33073,10 @@
       <c r="A19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="E19" s="8" t="s">
         <v>8</v>
       </c>
@@ -33086,10 +33088,10 @@
       <c r="A20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="35"/>
       <c r="E20" s="8" t="s">
         <v>0</v>
       </c>
@@ -33101,10 +33103,10 @@
       <c r="A21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="E21" s="8" t="s">
         <v>14</v>
       </c>
@@ -33116,10 +33118,10 @@
       <c r="A22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="35"/>
       <c r="E22" s="8" t="s">
         <v>18</v>
       </c>
@@ -33207,10 +33209,10 @@
       <c r="A31" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="33">
+      <c r="B31" s="36">
         <v>7</v>
       </c>
-      <c r="C31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="E31" s="19" t="s">
         <v>3</v>
       </c>
@@ -33222,10 +33224,10 @@
       <c r="A32" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="E32" s="21" t="s">
         <v>8</v>
       </c>
@@ -33237,10 +33239,10 @@
       <c r="A33" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="34"/>
+      <c r="C33" s="35"/>
       <c r="E33" s="21" t="s">
         <v>0</v>
       </c>
@@ -33252,10 +33254,10 @@
       <c r="A34" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="34"/>
+      <c r="C34" s="35"/>
       <c r="E34" s="21" t="s">
         <v>14</v>
       </c>
@@ -33267,10 +33269,10 @@
       <c r="A35" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="34"/>
+      <c r="C35" s="35"/>
       <c r="E35" s="21" t="s">
         <v>18</v>
       </c>
@@ -33356,10 +33358,10 @@
       <c r="A44" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="33">
+      <c r="B44" s="36">
         <v>8</v>
       </c>
-      <c r="C44" s="34"/>
+      <c r="C44" s="35"/>
       <c r="E44" s="19" t="s">
         <v>3</v>
       </c>
@@ -33371,10 +33373,10 @@
       <c r="A45" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="34"/>
+      <c r="C45" s="35"/>
       <c r="E45" s="21" t="s">
         <v>8</v>
       </c>
@@ -33386,10 +33388,10 @@
       <c r="A46" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="34"/>
+      <c r="C46" s="35"/>
       <c r="E46" s="21" t="s">
         <v>0</v>
       </c>
@@ -33401,10 +33403,10 @@
       <c r="A47" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="34"/>
+      <c r="C47" s="35"/>
       <c r="E47" s="21" t="s">
         <v>14</v>
       </c>
@@ -33416,10 +33418,10 @@
       <c r="A48" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="34"/>
+      <c r="C48" s="35"/>
       <c r="E48" s="21" t="s">
         <v>18</v>
       </c>
@@ -33463,50 +33465,50 @@
       <c r="A52" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="33">
+      <c r="B52" s="36">
         <v>9</v>
       </c>
-      <c r="C52" s="34"/>
+      <c r="C52" s="35"/>
       <c r="F52" s="13"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="34"/>
+      <c r="C53" s="35"/>
       <c r="F53" s="13"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1">
       <c r="A54" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="34"/>
+      <c r="C54" s="35"/>
       <c r="F54" s="13"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1">
       <c r="A55" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="34"/>
+      <c r="C55" s="35"/>
       <c r="F55" s="13"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
       <c r="A56" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="34"/>
+      <c r="C56" s="35"/>
       <c r="F56" s="13"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
@@ -36346,6 +36348,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
@@ -36356,21 +36373,6 @@
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -36387,7 +36389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -36406,10 +36408,10 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>10</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -36421,10 +36423,10 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -36436,10 +36438,10 @@
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
@@ -36449,10 +36451,10 @@
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -36464,10 +36466,10 @@
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
@@ -36511,10 +36513,10 @@
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="36">
         <v>11</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="35"/>
       <c r="E9" s="6" t="s">
         <v>3</v>
       </c>
@@ -36524,10 +36526,10 @@
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
@@ -36537,10 +36539,10 @@
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="E11" s="8" t="s">
         <v>0</v>
       </c>
@@ -36550,10 +36552,10 @@
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="E12" s="8" t="s">
         <v>14</v>
       </c>
@@ -36563,10 +36565,10 @@
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
@@ -36606,10 +36608,10 @@
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="36">
         <v>12</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="E17" s="6" t="s">
         <v>3</v>
       </c>
@@ -36619,10 +36621,10 @@
       <c r="A18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="E18" s="8" t="s">
         <v>8</v>
       </c>
@@ -36632,10 +36634,10 @@
       <c r="A19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="E19" s="8" t="s">
         <v>0</v>
       </c>
@@ -36645,10 +36647,10 @@
       <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="35"/>
       <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
@@ -36658,10 +36660,10 @@
       <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="E21" s="8" t="s">
         <v>18</v>
       </c>
@@ -36728,8 +36730,8 @@
       <c r="A28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="E28" s="8" t="s">
         <v>0</v>
       </c>
@@ -36739,8 +36741,8 @@
       <c r="A29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="E29" s="8" t="s">
         <v>14</v>
       </c>
@@ -36750,8 +36752,8 @@
       <c r="A30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="E30" s="8" t="s">
         <v>18</v>
       </c>
@@ -40644,6 +40646,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
@@ -40652,16 +40664,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -40694,10 +40696,10 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>13</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -40709,10 +40711,10 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -40724,10 +40726,10 @@
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
@@ -40739,10 +40741,10 @@
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -40754,10 +40756,10 @@
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
@@ -40811,10 +40813,10 @@
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="36">
         <v>14</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="E10" s="6" t="s">
         <v>3</v>
       </c>
@@ -40824,10 +40826,10 @@
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="35"/>
       <c r="E11" s="8" t="s">
         <v>8</v>
       </c>
@@ -40837,10 +40839,10 @@
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="35"/>
       <c r="E12" s="8" t="s">
         <v>0</v>
       </c>
@@ -40850,10 +40852,10 @@
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="35"/>
       <c r="E13" s="8" t="s">
         <v>14</v>
       </c>
@@ -40863,10 +40865,10 @@
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="34"/>
+      <c r="C14" s="35"/>
       <c r="E14" s="8" t="s">
         <v>18</v>
       </c>
@@ -40920,10 +40922,10 @@
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="36">
         <v>15</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="E19" s="6" t="s">
         <v>3</v>
       </c>
@@ -40933,10 +40935,10 @@
       <c r="A20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="35"/>
       <c r="E20" s="8" t="s">
         <v>8</v>
       </c>
@@ -40946,10 +40948,10 @@
       <c r="A21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="34"/>
+      <c r="C21" s="35"/>
       <c r="E21" s="8" t="s">
         <v>0</v>
       </c>
@@ -40959,10 +40961,10 @@
       <c r="A22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="34"/>
+      <c r="C22" s="35"/>
       <c r="E22" s="8" t="s">
         <v>14</v>
       </c>
@@ -40972,10 +40974,10 @@
       <c r="A23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="34"/>
+      <c r="C23" s="35"/>
       <c r="E23" s="8" t="s">
         <v>18</v>
       </c>
@@ -41029,10 +41031,10 @@
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="36">
         <v>16</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="E28" s="6" t="s">
         <v>3</v>
       </c>
@@ -41042,10 +41044,10 @@
       <c r="A29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="E29" s="8" t="s">
         <v>8</v>
       </c>
@@ -41055,10 +41057,10 @@
       <c r="A30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="E30" s="8" t="s">
         <v>0</v>
       </c>
@@ -41068,10 +41070,10 @@
       <c r="A31" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="C31" s="34"/>
+      <c r="C31" s="35"/>
       <c r="E31" s="8" t="s">
         <v>14</v>
       </c>
@@ -41081,10 +41083,10 @@
       <c r="A32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="34"/>
+      <c r="C32" s="35"/>
       <c r="E32" s="8" t="s">
         <v>18</v>
       </c>
@@ -45956,6 +45958,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
@@ -45966,16 +45978,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -45989,7 +45991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -46006,10 +46008,10 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="36">
         <v>17</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
@@ -46019,10 +46021,10 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -46032,10 +46034,10 @@
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
@@ -46045,10 +46047,10 @@
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="35"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -46058,10 +46060,10 @@
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="E5" s="8" t="s">
         <v>18</v>
       </c>
@@ -46167,10 +46169,10 @@
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="36">
         <v>18</v>
       </c>
-      <c r="C15" s="34"/>
+      <c r="C15" s="35"/>
       <c r="E15" s="6" t="s">
         <v>3</v>
       </c>
@@ -46180,10 +46182,10 @@
       <c r="A16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="35"/>
       <c r="E16" s="8" t="s">
         <v>8</v>
       </c>
@@ -46193,10 +46195,10 @@
       <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="E17" s="8" t="s">
         <v>0</v>
       </c>
@@ -46206,10 +46208,10 @@
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="E18" s="8" t="s">
         <v>14</v>
       </c>
@@ -46219,10 +46221,10 @@
       <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="E19" s="8" t="s">
         <v>18</v>
       </c>
@@ -46284,10 +46286,10 @@
       <c r="A25" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="33">
+      <c r="B25" s="36">
         <v>19</v>
       </c>
-      <c r="C25" s="34"/>
+      <c r="C25" s="35"/>
       <c r="E25" s="6" t="s">
         <v>3</v>
       </c>
@@ -46297,10 +46299,10 @@
       <c r="A26" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="35"/>
       <c r="E26" s="8" t="s">
         <v>8</v>
       </c>
@@ -46310,10 +46312,10 @@
       <c r="A27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="34"/>
+      <c r="C27" s="35"/>
       <c r="E27" s="8" t="s">
         <v>0</v>
       </c>
@@ -46323,10 +46325,10 @@
       <c r="A28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="34"/>
+      <c r="C28" s="35"/>
       <c r="E28" s="8" t="s">
         <v>14</v>
       </c>
@@ -46336,10 +46338,10 @@
       <c r="A29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="34"/>
+      <c r="C29" s="35"/>
       <c r="E29" s="8" t="s">
         <v>18</v>
       </c>
@@ -46408,8 +46410,8 @@
       <c r="A36" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
       <c r="E36" s="8" t="s">
         <v>0</v>
       </c>
@@ -46419,8 +46421,8 @@
       <c r="A37" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
       <c r="E37" s="8" t="s">
         <v>14</v>
       </c>
@@ -46430,8 +46432,8 @@
       <c r="A38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
       <c r="E38" s="8" t="s">
         <v>18</v>
       </c>
@@ -50324,6 +50326,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
@@ -50332,16 +50344,6 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>